<commit_message>
GeoData - Implemented Notebook for 4 datasets + added gene reference
</commit_message>
<xml_diff>
--- a/UITZOEKEN_Supplement/genesReferencesFeatureSetsNumbered.xlsx
+++ b/UITZOEKEN_Supplement/genesReferencesFeatureSetsNumbered.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\000_Projecten\HogeschoolRotterdam\ExploratoryDevelopmentCapstone\UITZOEKEN_Supplement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1078C3C5-2452-4AE9-B143-6B8A391487C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{220BEED5-F5B3-45A5-B8BE-2E9FE11A6363}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4380" yWindow="2316" windowWidth="17688" windowHeight="9924" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GeneAndReference" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2222" uniqueCount="413">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2224" uniqueCount="414">
   <si>
     <t>s10911-023-09540-2</t>
   </si>
@@ -1282,6 +1282,9 @@
   </si>
   <si>
     <t>AOC3</t>
+  </si>
+  <si>
+    <t>B7-H1</t>
   </si>
 </sst>
 </file>
@@ -1713,7 +1716,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:T294"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
@@ -10294,10 +10297,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08A0738F-DFD0-4775-9DE7-D468DC9E8D37}">
-  <dimension ref="C3:H61"/>
+  <dimension ref="C3:H62"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10732,113 +10735,122 @@
     </row>
     <row r="51" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C51" t="s">
-        <v>343</v>
-      </c>
-      <c r="D51" t="s">
-        <v>344</v>
-      </c>
+        <v>248</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>413</v>
+      </c>
+      <c r="E51" s="5"/>
     </row>
     <row r="52" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C52" t="s">
-        <v>284</v>
+        <v>343</v>
       </c>
       <c r="D52" t="s">
-        <v>127</v>
+        <v>344</v>
       </c>
     </row>
     <row r="53" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C53" t="s">
-        <v>272</v>
+        <v>284</v>
       </c>
       <c r="D53" t="s">
-        <v>21</v>
+        <v>127</v>
       </c>
     </row>
     <row r="54" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C54" t="s">
-        <v>252</v>
+        <v>272</v>
       </c>
       <c r="D54" t="s">
-        <v>254</v>
+        <v>21</v>
       </c>
     </row>
     <row r="55" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C55" t="s">
-        <v>335</v>
+        <v>252</v>
       </c>
       <c r="D55" t="s">
-        <v>336</v>
+        <v>254</v>
       </c>
     </row>
     <row r="56" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C56" t="s">
-        <v>318</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>317</v>
+        <v>335</v>
+      </c>
+      <c r="D56" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="57" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C57" t="s">
-        <v>296</v>
-      </c>
-      <c r="D57" t="s">
-        <v>193</v>
-      </c>
-      <c r="E57" t="s">
-        <v>194</v>
-      </c>
-      <c r="F57" t="s">
-        <v>195</v>
+        <v>318</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="58" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C58" t="s">
-        <v>273</v>
+        <v>296</v>
       </c>
       <c r="D58" t="s">
-        <v>46</v>
+        <v>193</v>
+      </c>
+      <c r="E58" t="s">
+        <v>194</v>
+      </c>
+      <c r="F58" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="59" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C59" t="s">
-        <v>302</v>
+        <v>273</v>
       </c>
       <c r="D59" t="s">
-        <v>243</v>
-      </c>
-      <c r="E59" t="s">
-        <v>244</v>
-      </c>
-      <c r="F59" t="s">
-        <v>245</v>
-      </c>
-      <c r="G59" t="s">
-        <v>246</v>
-      </c>
-      <c r="H59" t="s">
-        <v>127</v>
+        <v>46</v>
       </c>
     </row>
     <row r="60" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C60" t="s">
-        <v>291</v>
+        <v>302</v>
       </c>
       <c r="D60" t="s">
-        <v>292</v>
+        <v>243</v>
+      </c>
+      <c r="E60" t="s">
+        <v>244</v>
+      </c>
+      <c r="F60" t="s">
+        <v>245</v>
+      </c>
+      <c r="G60" t="s">
+        <v>246</v>
+      </c>
+      <c r="H60" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="61" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C61" t="s">
+        <v>291</v>
+      </c>
+      <c r="D61" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="62" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C62" t="s">
         <v>275</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D62" t="s">
         <v>276</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C5:H61">
-    <sortCondition ref="C5:C61"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C5:H62">
+    <sortCondition ref="C5:C62"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>